<commit_message>
Release 02/2020 - TYPO3 9.5
</commit_message>
<xml_diff>
--- a/web/fileadmin/vorlage.xlsx
+++ b/web/fileadmin/vorlage.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koop06\Desktop\DESK\Chancenportal.de Dateien\Pirmasens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sortmeyer/Library/Containers/com.microsoft.Excel/Data/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBE022B-00B6-C245-B44E-0206AC143A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8670" tabRatio="500"/>
+    <workbookView xWindow="29300" yWindow="-6340" windowWidth="63320" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exportEmFvLC.csv" sheetId="1" r:id="rId1"/>
@@ -20,12 +21,12 @@
     <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">#N/A</definedName>
     <definedName name="Excel_BuiltIn_Sheet_Title" localSheetId="0">"exportEmFvLC.csv"</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -150,9 +151,6 @@
     <t>ja</t>
   </si>
   <si>
-    <t>Datum (TT.MM.JJJ)</t>
-  </si>
-  <si>
     <t>Uhrzeit (HH:MM)</t>
   </si>
   <si>
@@ -214,9 +212,6 @@
   </si>
   <si>
     <t>Kooperationspartner für dieses Angebot</t>
-  </si>
-  <si>
-    <t>PLZ</t>
   </si>
   <si>
     <t>Referent/en, Berufsbezeichnung oder Qualifikation</t>
@@ -238,29 +233,13 @@
 </t>
   </si>
   <si>
-    <t>Dies ist ein Beispielangebot (vor Eingabe bitte Zeile löschen)</t>
-  </si>
-  <si>
-    <t>Datum (TT.MM.JJJ), 
-Für mehrere Daten eine neue Zeile mit selben Angebots-nummer verwenden</t>
-  </si>
-  <si>
     <t>Postleitzahl Stadt, Straße Nummer</t>
   </si>
   <si>
-    <t>Postleitzahl</t>
-  </si>
-  <si>
-    <t>Kurzbeschreibung, max. 200 Zeichen</t>
-  </si>
-  <si>
     <t>Adresse (Wo findet das Angebot statt?)*</t>
   </si>
   <si>
     <t>Teaser-Text (wird in der Listenansicht angezeigt)*</t>
-  </si>
-  <si>
-    <t>Freitext, max. 200 Zeichen</t>
   </si>
   <si>
     <t>33311 Güterlsoh, Carl-Bertelsmann-Straße 256</t>
@@ -297,11 +276,6 @@
     <t>mail@chancenportal.de</t>
   </si>
   <si>
-    <t>Langbeschreibung alkjdölakjlkdjsa lfakjd ölfdkjsafödsa ölkj fdsaölkj fdsa
-lköjsfölkjölskf j
-lkaölkjöklafd</t>
-  </si>
-  <si>
     <t>Max Mustermann</t>
   </si>
   <si>
@@ -309,13 +283,60 @@
   </si>
   <si>
     <t>Betreuung</t>
+  </si>
+  <si>
+    <t>Datum (TT.MM.JJJJ)</t>
+  </si>
+  <si>
+    <t>URL Anbieter</t>
+  </si>
+  <si>
+    <t>Eingagement möglich</t>
+  </si>
+  <si>
+    <t>www.chanchenportal.de</t>
+  </si>
+  <si>
+    <t>Beispielangebot (vor Import bitte löschen)</t>
+  </si>
+  <si>
+    <t>Datum (TT.MM.JJJJ), 
+Für mehrere Daten eine neue Zeile mit selber ID</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>Freitext, max. 200 Zeichen.</t>
+  </si>
+  <si>
+    <t>Kurzbeschreibung, max. 200 Zeichen
+Beim Import wird alles darüber liegende abgeschnitten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Langbeschreibung </t>
+  </si>
+  <si>
+    <t>Stadtteil*</t>
+  </si>
+  <si>
+    <t>Stadtteil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -357,6 +378,10 @@
       <color rgb="FFFF0000"/>
       <name val="Sans"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Sans"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -378,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -504,12 +529,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -561,26 +599,30 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,37 +1023,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AF149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="97" zoomScaleSheetLayoutView="10" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleSheetLayoutView="10" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="23.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.33203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
-    <col min="6" max="9" width="23.42578125" style="1"/>
-    <col min="10" max="10" width="23.42578125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="23.42578125" style="1"/>
-    <col min="13" max="13" width="50.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="62.5703125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="23.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="30.85546875" style="1" customWidth="1"/>
-    <col min="19" max="20" width="23.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="17.7109375" style="1" customWidth="1"/>
-    <col min="23" max="24" width="19.7109375" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="23.42578125" style="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="23.33203125" style="1"/>
+    <col min="10" max="10" width="23.33203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="23.33203125" style="1"/>
+    <col min="13" max="13" width="50.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="62.6640625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="23.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="30.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" style="1" customWidth="1"/>
+    <col min="19" max="20" width="23.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="17.83203125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="19.83203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="23.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="69" customHeight="1">
+    <row r="1" spans="1:32" ht="69" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1019,10 +1061,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>3</v>
@@ -1037,55 +1079,55 @@
         <v>4</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T1" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U1" s="13" t="s">
         <v>8</v>
       </c>
       <c r="V1" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="X1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="Z1" s="13" t="s">
         <v>12</v>
@@ -1102,46 +1144,52 @@
       <c r="AD1" s="16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" s="5" customFormat="1" ht="57.6" customHeight="1" thickBot="1">
+      <c r="AE1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="5" customFormat="1" ht="57.5" customHeight="1" thickBot="1">
       <c r="A2" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>42</v>
+      <c r="G2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>17</v>
@@ -1156,10 +1204,10 @@
         <v>19</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>17</v>
@@ -1194,35 +1242,43 @@
       <c r="AD2" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF2" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="23" customFormat="1" ht="28">
       <c r="A3" s="17">
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="27">
+        <v>43909</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="19">
-        <v>43539</v>
-      </c>
-      <c r="F3" s="20">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="20">
-        <v>0.5</v>
+      <c r="G3" s="27">
+        <v>43909</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K3" s="17">
         <v>33311</v>
@@ -1231,21 +1287,23 @@
         <v>29</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="25" t="s">
-        <v>80</v>
+      <c r="Q3" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="R3" s="17" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
+      <c r="T3" s="17">
+        <v>10</v>
+      </c>
       <c r="U3" s="17">
         <v>100</v>
       </c>
@@ -1253,79 +1311,89 @@
         <v>35</v>
       </c>
       <c r="W3" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X3" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB3" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC3" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE3" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD3" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="92.45" customHeight="1">
-      <c r="A4" s="23">
+    </row>
+    <row r="4" spans="1:32" s="23" customFormat="1">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="22">
-        <v>43544</v>
-      </c>
-      <c r="F4" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="21">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-    </row>
-    <row r="5" spans="1:30" ht="92.45" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="27">
+        <v>43911</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="27">
+        <v>43911</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+    </row>
+    <row r="5" spans="1:32" ht="92.5" customHeight="1">
+      <c r="A5" s="19"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
@@ -1348,16 +1416,18 @@
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
-    </row>
-    <row r="6" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+    </row>
+    <row r="6" spans="1:32" ht="92.5" customHeight="1">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
@@ -1380,16 +1450,18 @@
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
-    </row>
-    <row r="7" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+    </row>
+    <row r="7" spans="1:32" ht="92.5" customHeight="1">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
@@ -1412,16 +1484,18 @@
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
-    </row>
-    <row r="8" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+    </row>
+    <row r="8" spans="1:32" ht="92.5" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -1444,16 +1518,18 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
-    </row>
-    <row r="9" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+    </row>
+    <row r="9" spans="1:32" ht="92.5" customHeight="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -1476,16 +1552,18 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
-    </row>
-    <row r="10" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+    </row>
+    <row r="10" spans="1:32" ht="92.5" customHeight="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1508,16 +1586,18 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
-    </row>
-    <row r="11" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+    </row>
+    <row r="11" spans="1:32" ht="92.5" customHeight="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1540,16 +1620,18 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
-    </row>
-    <row r="12" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+    </row>
+    <row r="12" spans="1:32" ht="92.5" customHeight="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -1572,16 +1654,18 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
-    </row>
-    <row r="13" spans="1:30" ht="92.45" customHeight="1">
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+    </row>
+    <row r="13" spans="1:32" ht="92.5" customHeight="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -1604,191 +1688,220 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
-    </row>
-    <row r="14" spans="1:30" ht="92.45" customHeight="1"/>
-    <row r="15" spans="1:30" ht="92.45" customHeight="1"/>
-    <row r="16" spans="1:30" ht="92.45" customHeight="1"/>
-    <row r="17" ht="92.45" customHeight="1"/>
-    <row r="18" ht="92.45" customHeight="1"/>
-    <row r="19" ht="92.45" customHeight="1"/>
-    <row r="20" ht="92.45" customHeight="1"/>
-    <row r="21" ht="92.45" customHeight="1"/>
-    <row r="22" ht="92.45" customHeight="1"/>
-    <row r="23" ht="92.45" customHeight="1"/>
-    <row r="24" ht="92.45" customHeight="1"/>
-    <row r="25" ht="92.45" customHeight="1"/>
-    <row r="26" ht="92.45" customHeight="1"/>
-    <row r="27" ht="92.45" customHeight="1"/>
-    <row r="28" ht="92.45" customHeight="1"/>
-    <row r="29" ht="92.45" customHeight="1"/>
-    <row r="30" ht="92.45" customHeight="1"/>
-    <row r="31" ht="92.45" customHeight="1"/>
-    <row r="32" ht="92.45" customHeight="1"/>
-    <row r="33" ht="92.45" customHeight="1"/>
-    <row r="34" ht="92.45" customHeight="1"/>
-    <row r="35" ht="92.45" customHeight="1"/>
-    <row r="36" ht="92.45" customHeight="1"/>
-    <row r="37" ht="92.45" customHeight="1"/>
-    <row r="38" ht="92.45" customHeight="1"/>
-    <row r="39" ht="92.45" customHeight="1"/>
-    <row r="40" ht="92.45" customHeight="1"/>
-    <row r="41" ht="92.45" customHeight="1"/>
-    <row r="42" ht="92.45" customHeight="1"/>
-    <row r="43" ht="92.45" customHeight="1"/>
-    <row r="44" ht="92.45" customHeight="1"/>
-    <row r="45" ht="92.45" customHeight="1"/>
-    <row r="46" ht="92.45" customHeight="1"/>
-    <row r="47" ht="92.45" customHeight="1"/>
-    <row r="48" ht="92.45" customHeight="1"/>
-    <row r="49" ht="92.45" customHeight="1"/>
-    <row r="50" ht="92.45" customHeight="1"/>
-    <row r="51" ht="92.45" customHeight="1"/>
-    <row r="52" ht="92.45" customHeight="1"/>
-    <row r="53" ht="92.45" customHeight="1"/>
-    <row r="54" ht="92.45" customHeight="1"/>
-    <row r="55" ht="92.45" customHeight="1"/>
-    <row r="56" ht="92.45" customHeight="1"/>
-    <row r="57" ht="92.45" customHeight="1"/>
-    <row r="58" ht="92.45" customHeight="1"/>
-    <row r="59" ht="92.45" customHeight="1"/>
-    <row r="60" ht="92.45" customHeight="1"/>
-    <row r="61" ht="92.45" customHeight="1"/>
-    <row r="62" ht="92.45" customHeight="1"/>
-    <row r="63" ht="92.45" customHeight="1"/>
-    <row r="64" ht="92.45" customHeight="1"/>
-    <row r="65" ht="92.45" customHeight="1"/>
-    <row r="66" ht="92.45" customHeight="1"/>
-    <row r="67" ht="92.45" customHeight="1"/>
-    <row r="68" ht="92.45" customHeight="1"/>
-    <row r="69" ht="92.45" customHeight="1"/>
-    <row r="70" ht="92.45" customHeight="1"/>
-    <row r="71" ht="92.45" customHeight="1"/>
-    <row r="72" ht="92.45" customHeight="1"/>
-    <row r="73" ht="92.45" customHeight="1"/>
-    <row r="74" ht="92.45" customHeight="1"/>
-    <row r="75" ht="92.45" customHeight="1"/>
-    <row r="76" ht="92.45" customHeight="1"/>
-    <row r="77" ht="92.45" customHeight="1"/>
-    <row r="78" ht="92.45" customHeight="1"/>
-    <row r="79" ht="92.45" customHeight="1"/>
-    <row r="80" ht="92.45" customHeight="1"/>
-    <row r="81" ht="92.45" customHeight="1"/>
-    <row r="82" ht="92.45" customHeight="1"/>
-    <row r="83" ht="92.45" customHeight="1"/>
-    <row r="84" ht="92.45" customHeight="1"/>
-    <row r="85" ht="92.45" customHeight="1"/>
-    <row r="86" ht="92.45" customHeight="1"/>
-    <row r="87" ht="92.45" customHeight="1"/>
-    <row r="88" ht="92.45" customHeight="1"/>
-    <row r="89" ht="92.45" customHeight="1"/>
-    <row r="90" ht="92.45" customHeight="1"/>
-    <row r="91" ht="92.45" customHeight="1"/>
-    <row r="92" ht="92.45" customHeight="1"/>
-    <row r="93" ht="92.45" customHeight="1"/>
-    <row r="94" ht="92.45" customHeight="1"/>
-    <row r="95" ht="92.45" customHeight="1"/>
-    <row r="96" ht="92.45" customHeight="1"/>
-    <row r="97" ht="92.45" customHeight="1"/>
-    <row r="98" ht="92.45" customHeight="1"/>
-    <row r="99" ht="92.45" customHeight="1"/>
-    <row r="100" ht="92.45" customHeight="1"/>
-    <row r="101" ht="92.45" customHeight="1"/>
-    <row r="102" ht="92.45" customHeight="1"/>
-    <row r="103" ht="92.45" customHeight="1"/>
-    <row r="104" ht="92.45" customHeight="1"/>
-    <row r="105" ht="92.45" customHeight="1"/>
-    <row r="106" ht="92.45" customHeight="1"/>
-    <row r="107" ht="92.45" customHeight="1"/>
-    <row r="108" ht="92.45" customHeight="1"/>
-    <row r="109" ht="92.45" customHeight="1"/>
-    <row r="110" ht="92.45" customHeight="1"/>
-    <row r="111" ht="92.45" customHeight="1"/>
-    <row r="112" ht="92.45" customHeight="1"/>
-    <row r="113" ht="92.45" customHeight="1"/>
-    <row r="114" ht="92.45" customHeight="1"/>
-    <row r="115" ht="92.45" customHeight="1"/>
-    <row r="116" ht="92.45" customHeight="1"/>
-    <row r="117" ht="92.45" customHeight="1"/>
-    <row r="118" ht="92.45" customHeight="1"/>
-    <row r="119" ht="92.45" customHeight="1"/>
-    <row r="120" ht="92.45" customHeight="1"/>
-    <row r="121" ht="92.45" customHeight="1"/>
-    <row r="122" ht="92.45" customHeight="1"/>
-    <row r="123" ht="92.45" customHeight="1"/>
-    <row r="124" ht="92.45" customHeight="1"/>
-    <row r="125" ht="92.45" customHeight="1"/>
-    <row r="126" ht="92.45" customHeight="1"/>
-    <row r="127" ht="92.45" customHeight="1"/>
-    <row r="128" ht="92.45" customHeight="1"/>
-    <row r="129" ht="92.45" customHeight="1"/>
-    <row r="130" ht="92.45" customHeight="1"/>
-    <row r="131" ht="92.45" customHeight="1"/>
-    <row r="132" ht="92.45" customHeight="1"/>
-    <row r="133" ht="92.45" customHeight="1"/>
-    <row r="134" ht="92.45" customHeight="1"/>
-    <row r="135" ht="92.45" customHeight="1"/>
-    <row r="136" ht="92.45" customHeight="1"/>
-    <row r="137" ht="92.45" customHeight="1"/>
-    <row r="138" ht="92.45" customHeight="1"/>
-    <row r="139" ht="92.45" customHeight="1"/>
-    <row r="140" ht="92.45" customHeight="1"/>
-    <row r="141" ht="92.45" customHeight="1"/>
-    <row r="142" ht="92.45" customHeight="1"/>
-    <row r="143" ht="92.45" customHeight="1"/>
-    <row r="144" ht="92.45" customHeight="1"/>
-    <row r="145" ht="92.45" customHeight="1"/>
-    <row r="146" ht="92.45" customHeight="1"/>
-    <row r="147" ht="92.45" customHeight="1"/>
-    <row r="148" ht="92.45" customHeight="1"/>
-    <row r="149" ht="92.45" customHeight="1"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+    </row>
+    <row r="14" spans="1:32" ht="92.5" customHeight="1">
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:32" ht="92.5" customHeight="1">
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:32" ht="92.5" customHeight="1">
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="5:8" ht="92.5" customHeight="1">
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="5:8" ht="92.5" customHeight="1">
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="20" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="21" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="22" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="23" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="24" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="25" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="26" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="27" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="28" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="29" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="30" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="31" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="32" spans="5:8" ht="92.5" customHeight="1"/>
+    <row r="33" ht="92.5" customHeight="1"/>
+    <row r="34" ht="92.5" customHeight="1"/>
+    <row r="35" ht="92.5" customHeight="1"/>
+    <row r="36" ht="92.5" customHeight="1"/>
+    <row r="37" ht="92.5" customHeight="1"/>
+    <row r="38" ht="92.5" customHeight="1"/>
+    <row r="39" ht="92.5" customHeight="1"/>
+    <row r="40" ht="92.5" customHeight="1"/>
+    <row r="41" ht="92.5" customHeight="1"/>
+    <row r="42" ht="92.5" customHeight="1"/>
+    <row r="43" ht="92.5" customHeight="1"/>
+    <row r="44" ht="92.5" customHeight="1"/>
+    <row r="45" ht="92.5" customHeight="1"/>
+    <row r="46" ht="92.5" customHeight="1"/>
+    <row r="47" ht="92.5" customHeight="1"/>
+    <row r="48" ht="92.5" customHeight="1"/>
+    <row r="49" ht="92.5" customHeight="1"/>
+    <row r="50" ht="92.5" customHeight="1"/>
+    <row r="51" ht="92.5" customHeight="1"/>
+    <row r="52" ht="92.5" customHeight="1"/>
+    <row r="53" ht="92.5" customHeight="1"/>
+    <row r="54" ht="92.5" customHeight="1"/>
+    <row r="55" ht="92.5" customHeight="1"/>
+    <row r="56" ht="92.5" customHeight="1"/>
+    <row r="57" ht="92.5" customHeight="1"/>
+    <row r="58" ht="92.5" customHeight="1"/>
+    <row r="59" ht="92.5" customHeight="1"/>
+    <row r="60" ht="92.5" customHeight="1"/>
+    <row r="61" ht="92.5" customHeight="1"/>
+    <row r="62" ht="92.5" customHeight="1"/>
+    <row r="63" ht="92.5" customHeight="1"/>
+    <row r="64" ht="92.5" customHeight="1"/>
+    <row r="65" ht="92.5" customHeight="1"/>
+    <row r="66" ht="92.5" customHeight="1"/>
+    <row r="67" ht="92.5" customHeight="1"/>
+    <row r="68" ht="92.5" customHeight="1"/>
+    <row r="69" ht="92.5" customHeight="1"/>
+    <row r="70" ht="92.5" customHeight="1"/>
+    <row r="71" ht="92.5" customHeight="1"/>
+    <row r="72" ht="92.5" customHeight="1"/>
+    <row r="73" ht="92.5" customHeight="1"/>
+    <row r="74" ht="92.5" customHeight="1"/>
+    <row r="75" ht="92.5" customHeight="1"/>
+    <row r="76" ht="92.5" customHeight="1"/>
+    <row r="77" ht="92.5" customHeight="1"/>
+    <row r="78" ht="92.5" customHeight="1"/>
+    <row r="79" ht="92.5" customHeight="1"/>
+    <row r="80" ht="92.5" customHeight="1"/>
+    <row r="81" ht="92.5" customHeight="1"/>
+    <row r="82" ht="92.5" customHeight="1"/>
+    <row r="83" ht="92.5" customHeight="1"/>
+    <row r="84" ht="92.5" customHeight="1"/>
+    <row r="85" ht="92.5" customHeight="1"/>
+    <row r="86" ht="92.5" customHeight="1"/>
+    <row r="87" ht="92.5" customHeight="1"/>
+    <row r="88" ht="92.5" customHeight="1"/>
+    <row r="89" ht="92.5" customHeight="1"/>
+    <row r="90" ht="92.5" customHeight="1"/>
+    <row r="91" ht="92.5" customHeight="1"/>
+    <row r="92" ht="92.5" customHeight="1"/>
+    <row r="93" ht="92.5" customHeight="1"/>
+    <row r="94" ht="92.5" customHeight="1"/>
+    <row r="95" ht="92.5" customHeight="1"/>
+    <row r="96" ht="92.5" customHeight="1"/>
+    <row r="97" ht="92.5" customHeight="1"/>
+    <row r="98" ht="92.5" customHeight="1"/>
+    <row r="99" ht="92.5" customHeight="1"/>
+    <row r="100" ht="92.5" customHeight="1"/>
+    <row r="101" ht="92.5" customHeight="1"/>
+    <row r="102" ht="92.5" customHeight="1"/>
+    <row r="103" ht="92.5" customHeight="1"/>
+    <row r="104" ht="92.5" customHeight="1"/>
+    <row r="105" ht="92.5" customHeight="1"/>
+    <row r="106" ht="92.5" customHeight="1"/>
+    <row r="107" ht="92.5" customHeight="1"/>
+    <row r="108" ht="92.5" customHeight="1"/>
+    <row r="109" ht="92.5" customHeight="1"/>
+    <row r="110" ht="92.5" customHeight="1"/>
+    <row r="111" ht="92.5" customHeight="1"/>
+    <row r="112" ht="92.5" customHeight="1"/>
+    <row r="113" ht="92.5" customHeight="1"/>
+    <row r="114" ht="92.5" customHeight="1"/>
+    <row r="115" ht="92.5" customHeight="1"/>
+    <row r="116" ht="92.5" customHeight="1"/>
+    <row r="117" ht="92.5" customHeight="1"/>
+    <row r="118" ht="92.5" customHeight="1"/>
+    <row r="119" ht="92.5" customHeight="1"/>
+    <row r="120" ht="92.5" customHeight="1"/>
+    <row r="121" ht="92.5" customHeight="1"/>
+    <row r="122" ht="92.5" customHeight="1"/>
+    <row r="123" ht="92.5" customHeight="1"/>
+    <row r="124" ht="92.5" customHeight="1"/>
+    <row r="125" ht="92.5" customHeight="1"/>
+    <row r="126" ht="92.5" customHeight="1"/>
+    <row r="127" ht="92.5" customHeight="1"/>
+    <row r="128" ht="92.5" customHeight="1"/>
+    <row r="129" ht="92.5" customHeight="1"/>
+    <row r="130" ht="92.5" customHeight="1"/>
+    <row r="131" ht="92.5" customHeight="1"/>
+    <row r="132" ht="92.5" customHeight="1"/>
+    <row r="133" ht="92.5" customHeight="1"/>
+    <row r="134" ht="92.5" customHeight="1"/>
+    <row r="135" ht="92.5" customHeight="1"/>
+    <row r="136" ht="92.5" customHeight="1"/>
+    <row r="137" ht="92.5" customHeight="1"/>
+    <row r="138" ht="92.5" customHeight="1"/>
+    <row r="139" ht="92.5" customHeight="1"/>
+    <row r="140" ht="92.5" customHeight="1"/>
+    <row r="141" ht="92.5" customHeight="1"/>
+    <row r="142" ht="92.5" customHeight="1"/>
+    <row r="143" ht="92.5" customHeight="1"/>
+    <row r="144" ht="92.5" customHeight="1"/>
+    <row r="145" ht="92.5" customHeight="1"/>
+    <row r="146" ht="92.5" customHeight="1"/>
+    <row r="147" ht="92.5" customHeight="1"/>
+    <row r="148" ht="92.5" customHeight="1"/>
+    <row r="149" ht="92.5" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AD3" r:id="rId1"/>
+    <hyperlink ref="AD3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="AE3" r:id="rId2" xr:uid="{6E7ADD13-D156-AD4C-B626-B993A7CBEC87}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" cellComments="atEnd" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" cellComments="atEnd" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$11:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$36:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>V3:V1048576</xm:sqref>
+          <xm:sqref>V3:V1048576 AF3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$41:$A$43</xm:f>
           </x14:formula1>
           <xm:sqref>W3:W1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$48:$A$50</xm:f>
           </x14:formula1>
           <xm:sqref>X3:X1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$54:$A$55</xm:f>
           </x14:formula1>
           <xm:sqref>Z3:Z1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$3:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>C3:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>'Felder Einfachauswahl'!$A$20:$A$31</xm:f>
           </x14:formula1>
@@ -1801,14 +1914,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="3" t="s">
@@ -1817,7 +1930,7 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1832,7 +1945,7 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -1842,27 +1955,27 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -1907,27 +2020,27 @@
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:1">
@@ -1992,12 +2105,12 @@
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -2021,6 +2134,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E09C5FE4D933424F819685CC62690DA1" ma:contentTypeVersion="1" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d8d93c2a9595ab8b31e2b63a758c4eaa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180f2ef5-dffa-40a5-8238-756645e0cabf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="36292cf951d0fe117e8d2b237c5c783e" ns2:_="">
     <xsd:import namespace="180f2ef5-dffa-40a5-8238-756645e0cabf"/>
@@ -2160,12 +2279,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{025A26FE-2710-4C26-8E52-BAAA444F1BAD}">
   <ds:schemaRefs>
@@ -2175,6 +2288,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13129218-3E01-437D-BF90-FDE09A5B103D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="180f2ef5-dffa-40a5-8238-756645e0cabf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F90F728-0421-4894-B295-DE19C3CF7EDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2190,20 +2319,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13129218-3E01-437D-BF90-FDE09A5B103D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="180f2ef5-dffa-40a5-8238-756645e0cabf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>